<commit_message>
Finished exercise and ran successfully.
</commit_message>
<xml_diff>
--- a/Input/Acquisitions.xlsx
+++ b/Input/Acquisitions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20406"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ganga.y\Downloads\Excel Data Consolidation_1\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ron.hiscock\Documents\UiPath\Excel Example 3 automation\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F2C9C37-983E-4231-9F81-E978896D7B53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75D1E097-CCE5-4EBC-888D-123C16514B16}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2784" yWindow="3528" windowWidth="19812" windowHeight="8832" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2790" yWindow="3525" windowWidth="19815" windowHeight="8835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Acquisitions" sheetId="1" r:id="rId1"/>
@@ -394,15 +394,15 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -416,7 +416,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>5453474984</v>
       </c>
@@ -430,7 +430,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1670739277</v>
       </c>
@@ -444,7 +444,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>6886493954</v>
       </c>
@@ -458,7 +458,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1940537091</v>
       </c>
@@ -472,7 +472,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>344493736</v>
       </c>
@@ -486,7 +486,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1325892864</v>
       </c>
@@ -500,7 +500,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6407345657</v>
       </c>
@@ -514,7 +514,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>696810766</v>
       </c>
@@ -528,7 +528,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6334443718</v>
       </c>
@@ -542,7 +542,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1535158254</v>
       </c>
@@ -556,7 +556,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>3899360176</v>
       </c>
@@ -570,7 +570,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1821674998</v>
       </c>
@@ -584,7 +584,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1247112419</v>
       </c>
@@ -598,7 +598,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2589735420</v>
       </c>
@@ -612,7 +612,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2873399350</v>
       </c>
@@ -626,7 +626,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2655378228</v>
       </c>
@@ -640,7 +640,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2922933540</v>
       </c>
@@ -654,7 +654,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>9030362344</v>
       </c>
@@ -668,7 +668,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2070082886</v>
       </c>
@@ -682,7 +682,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>8521461724</v>
       </c>
@@ -696,7 +696,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2108308179</v>
       </c>
@@ -710,7 +710,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>4088197331</v>
       </c>
@@ -724,7 +724,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>3859776225</v>
       </c>
@@ -738,7 +738,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>6476113995</v>
       </c>
@@ -752,7 +752,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>7046151500</v>
       </c>
@@ -766,7 +766,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>3798116537</v>
       </c>
@@ -780,7 +780,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>6238641630</v>
       </c>
@@ -794,7 +794,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>9701622924</v>
       </c>
@@ -808,7 +808,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>8393159088</v>
       </c>
@@ -822,7 +822,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>4350648720</v>
       </c>
@@ -836,7 +836,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1189483470</v>
       </c>
@@ -850,7 +850,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>3235131803</v>
       </c>
@@ -864,7 +864,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2760484642</v>
       </c>
@@ -878,7 +878,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>8535017088</v>
       </c>
@@ -892,7 +892,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>301391492</v>
       </c>
@@ -906,7 +906,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>5796214458</v>
       </c>
@@ -920,7 +920,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>6093866711</v>
       </c>
@@ -934,7 +934,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>7574908423</v>
       </c>
@@ -948,7 +948,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>4581808517</v>
       </c>
@@ -962,7 +962,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>6690655378</v>
       </c>
@@ -976,7 +976,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>6087181936</v>
       </c>
@@ -990,7 +990,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>5706842005</v>
       </c>
@@ -1004,7 +1004,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>5834578709</v>
       </c>
@@ -1018,7 +1018,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>1995748856</v>
       </c>
@@ -1032,7 +1032,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>5656598490</v>
       </c>
@@ -1046,7 +1046,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>710626128</v>
       </c>
@@ -1060,7 +1060,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>1557872693</v>
       </c>
@@ -1074,7 +1074,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>7780238133</v>
       </c>
@@ -1088,7 +1088,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>9191615273</v>
       </c>
@@ -1102,7 +1102,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>2528259912</v>
       </c>
@@ -1116,7 +1116,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>2599166755</v>
       </c>
@@ -1130,7 +1130,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>4014088315</v>
       </c>
@@ -1144,7 +1144,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>4796405029</v>
       </c>
@@ -1158,7 +1158,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>4396103791</v>
       </c>
@@ -1172,7 +1172,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>5712180893</v>
       </c>
@@ -1186,7 +1186,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>9389160868</v>
       </c>
@@ -1200,7 +1200,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>7900224879</v>
       </c>
@@ -1214,7 +1214,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>6076769556</v>
       </c>
@@ -1228,7 +1228,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>8145965305</v>
       </c>
@@ -1242,7 +1242,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>1640688575</v>
       </c>
@@ -1256,7 +1256,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>819688255</v>
       </c>
@@ -1270,7 +1270,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>7059882652</v>
       </c>
@@ -1284,7 +1284,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>2063332893</v>
       </c>
@@ -1298,7 +1298,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>3050268903</v>
       </c>
@@ -1312,7 +1312,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>3272744246</v>
       </c>
@@ -1326,7 +1326,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>9699365891</v>
       </c>
@@ -1340,7 +1340,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>4081538748</v>
       </c>
@@ -1354,7 +1354,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>9167827396</v>
       </c>
@@ -1368,7 +1368,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>4314582598</v>
       </c>
@@ -1382,7 +1382,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>7275801788</v>
       </c>
@@ -1396,7 +1396,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>7951469064</v>
       </c>
@@ -1410,7 +1410,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>9837166255</v>
       </c>
@@ -1424,7 +1424,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>7453425369</v>
       </c>
@@ -1438,7 +1438,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>5800814438</v>
       </c>
@@ -1452,7 +1452,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>6382736869</v>
       </c>
@@ -1466,7 +1466,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>3324963692</v>
       </c>
@@ -1480,7 +1480,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>4371610407</v>
       </c>
@@ -1494,7 +1494,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>8767288098</v>
       </c>
@@ -1508,7 +1508,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>9160470472</v>
       </c>
@@ -1522,7 +1522,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>2145703919</v>
       </c>
@@ -1536,7 +1536,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>7628380553</v>
       </c>
@@ -1550,7 +1550,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>4921748485</v>
       </c>
@@ -1564,7 +1564,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>8014752845</v>
       </c>
@@ -1578,7 +1578,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>3549956879</v>
       </c>
@@ -1592,7 +1592,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>8592887088</v>
       </c>
@@ -1606,7 +1606,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>3063442179</v>
       </c>
@@ -1620,7 +1620,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>8285066584</v>
       </c>
@@ -1634,7 +1634,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>8197575841</v>
       </c>
@@ -1648,7 +1648,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>7491619375</v>
       </c>
@@ -1662,7 +1662,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>9212725452</v>
       </c>
@@ -1676,7 +1676,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>6654139710</v>
       </c>
@@ -1690,7 +1690,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>9397591136</v>
       </c>
@@ -1704,7 +1704,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>4448112171</v>
       </c>
@@ -1718,7 +1718,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>8125148091</v>
       </c>
@@ -1732,7 +1732,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>8743510414</v>
       </c>
@@ -1746,7 +1746,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>584836743</v>
       </c>
@@ -1760,7 +1760,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>2584752895</v>
       </c>
@@ -1774,7 +1774,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>4306664738</v>
       </c>
@@ -1788,7 +1788,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>6071010616</v>
       </c>
@@ -1802,7 +1802,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>7857668110</v>
       </c>

</xml_diff>

<commit_message>
Added an excel process scope to make the program headless.
</commit_message>
<xml_diff>
--- a/Input/Acquisitions.xlsx
+++ b/Input/Acquisitions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ron.hiscock\Documents\UiPath\Excel Example 3 automation\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75D1E097-CCE5-4EBC-888D-123C16514B16}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{923F7084-EE88-45CB-A175-C1DC09962C2A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2790" yWindow="3525" windowWidth="19815" windowHeight="8835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1822,6 +1822,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="34d2ab49-b14c-40af-8c3f-b2a27eb69e13" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="328982d7-d2af-46e2-9ab4-9b069b3e82d0">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B47328280439544AB5C41C56297158F8" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="50e5b6106be706602d4845c0a9b0c3da">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="825ee06b-ca9e-4fae-a309-081319cc5c11" xmlns:ns3="328982d7-d2af-46e2-9ab4-9b069b3e82d0" xmlns:ns4="34d2ab49-b14c-40af-8c3f-b2a27eb69e13" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f931b1fd44a63a33fbd98fb4653837c7" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="825ee06b-ca9e-4fae-a309-081319cc5c11"/>
@@ -2063,27 +2083,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="34d2ab49-b14c-40af-8c3f-b2a27eb69e13" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="328982d7-d2af-46e2-9ab4-9b069b3e82d0">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7AB9A8E1-E04D-4628-9179-505861E9CEB4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB5C6EBF-4902-4536-B72A-0466FB8219D8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="34d2ab49-b14c-40af-8c3f-b2a27eb69e13"/>
+    <ds:schemaRef ds:uri="328982d7-d2af-46e2-9ab4-9b069b3e82d0"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CFAAA239-A697-4242-BDF8-153903A180C6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2101,23 +2120,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB5C6EBF-4902-4536-B72A-0466FB8219D8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="34d2ab49-b14c-40af-8c3f-b2a27eb69e13"/>
-    <ds:schemaRef ds:uri="328982d7-d2af-46e2-9ab4-9b069b3e82d0"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7AB9A8E1-E04D-4628-9179-505861E9CEB4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>